<commit_message>
Adding LSBFS algorithm and updated test results
</commit_message>
<xml_diff>
--- a/FinalPresentation/Test Results.xlsx
+++ b/FinalPresentation/Test Results.xlsx
@@ -132,7 +132,7 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$L$3:$O$3</c:f>
+              <c:f>Sheet1!$A$26:$D$26</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -152,7 +152,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$4:$O$4</c:f>
+              <c:f>Sheet1!$A$27:$D$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -287,7 +287,7 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$Q$3:$T$3</c:f>
+              <c:f>Sheet1!$F$26:$I$26</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -307,7 +307,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$4:$T$4</c:f>
+              <c:f>Sheet1!$F$27:$I$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -410,15 +410,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>0</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -440,15 +440,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -756,10 +756,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U21"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -767,7 +767,7 @@
     <col min="5" max="5" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -775,7 +775,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -800,14 +800,8 @@
       <c r="I2" t="s">
         <v>3</v>
       </c>
-      <c r="L2" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>21</v>
       </c>
@@ -838,32 +832,8 @@
       <c r="J3" t="s">
         <v>4</v>
       </c>
-      <c r="L3" t="s">
-        <v>0</v>
-      </c>
-      <c r="M3" t="s">
-        <v>1</v>
-      </c>
-      <c r="N3" t="s">
-        <v>2</v>
-      </c>
-      <c r="O3" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>0</v>
-      </c>
-      <c r="R3" t="s">
-        <v>1</v>
-      </c>
-      <c r="S3" t="s">
-        <v>2</v>
-      </c>
-      <c r="T3" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>23</v>
       </c>
@@ -894,146 +864,182 @@
       <c r="J4" t="s">
         <v>4</v>
       </c>
-      <c r="L4">
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5">
+        <v>27</v>
+      </c>
+      <c r="B5">
+        <v>568</v>
+      </c>
+      <c r="C5">
+        <v>42</v>
+      </c>
+      <c r="D5">
+        <v>231</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>292</v>
+      </c>
+      <c r="G5">
+        <v>426</v>
+      </c>
+      <c r="H5">
+        <v>131</v>
+      </c>
+      <c r="I5">
+        <v>598</v>
+      </c>
+      <c r="J5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>570</v>
+      </c>
+      <c r="C6">
+        <v>51</v>
+      </c>
+      <c r="D6">
+        <v>244</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>296</v>
+      </c>
+      <c r="G6">
+        <v>439</v>
+      </c>
+      <c r="H6">
+        <v>116</v>
+      </c>
+      <c r="I6">
+        <v>705</v>
+      </c>
+      <c r="J6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7">
+        <v>21</v>
+      </c>
+      <c r="B7">
+        <v>522</v>
+      </c>
+      <c r="C7">
+        <v>43</v>
+      </c>
+      <c r="D7">
+        <v>556</v>
+      </c>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>294</v>
+      </c>
+      <c r="G7">
+        <v>217</v>
+      </c>
+      <c r="H7">
+        <v>207</v>
+      </c>
+      <c r="I7">
+        <v>856</v>
+      </c>
+      <c r="J7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>3</v>
+      </c>
+      <c r="F26" t="s">
+        <v>0</v>
+      </c>
+      <c r="G26" t="s">
+        <v>1</v>
+      </c>
+      <c r="H26" t="s">
+        <v>2</v>
+      </c>
+      <c r="I26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27">
         <f>AVERAGE(A3:A7)</f>
         <v>22.4</v>
       </c>
-      <c r="M4">
+      <c r="B27">
         <f>AVERAGE(B3:B7)</f>
         <v>555</v>
       </c>
-      <c r="N4">
+      <c r="C27">
         <f>AVERAGE(C3:C7)</f>
         <v>45</v>
       </c>
-      <c r="O4">
+      <c r="D27">
         <f>AVERAGE(D3:D7)</f>
         <v>510.2</v>
       </c>
-      <c r="P4" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q4">
+      <c r="E27" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27">
         <f>AVERAGE(F3:F7)</f>
         <v>293</v>
       </c>
-      <c r="R4">
+      <c r="G27">
         <f>AVERAGE(G3:G7)</f>
         <v>404.8</v>
       </c>
-      <c r="S4">
+      <c r="H27">
         <f>AVERAGE(H3:H7)</f>
         <v>150.80000000000001</v>
       </c>
-      <c r="T4">
+      <c r="I27">
         <f>AVERAGE(I3:I7)</f>
         <v>631</v>
       </c>
-      <c r="U4" t="s">
+      <c r="J27" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
-      <c r="A5">
-        <v>27</v>
-      </c>
-      <c r="B5">
-        <v>568</v>
-      </c>
-      <c r="C5">
-        <v>42</v>
-      </c>
-      <c r="D5">
-        <v>231</v>
-      </c>
-      <c r="E5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5">
-        <v>292</v>
-      </c>
-      <c r="G5">
-        <v>426</v>
-      </c>
-      <c r="H5">
-        <v>131</v>
-      </c>
-      <c r="I5">
-        <v>598</v>
-      </c>
-      <c r="J5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21">
-      <c r="A6">
-        <v>20</v>
-      </c>
-      <c r="B6">
-        <v>570</v>
-      </c>
-      <c r="C6">
-        <v>51</v>
-      </c>
-      <c r="D6">
-        <v>244</v>
-      </c>
-      <c r="E6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6">
-        <v>296</v>
-      </c>
-      <c r="G6">
-        <v>439</v>
-      </c>
-      <c r="H6">
-        <v>116</v>
-      </c>
-      <c r="I6">
-        <v>705</v>
-      </c>
-      <c r="J6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21">
-      <c r="A7">
-        <v>21</v>
-      </c>
-      <c r="B7">
-        <v>522</v>
-      </c>
-      <c r="C7">
-        <v>43</v>
-      </c>
-      <c r="D7">
-        <v>556</v>
-      </c>
-      <c r="E7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7">
-        <v>294</v>
-      </c>
-      <c r="G7">
-        <v>217</v>
-      </c>
-      <c r="H7">
-        <v>207</v>
-      </c>
-      <c r="I7">
-        <v>856</v>
-      </c>
-      <c r="J7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="12:20">
-      <c r="L21" t="s">
+    <row r="44" spans="1:9">
+      <c r="A44" t="s">
         <v>9</v>
       </c>
-      <c r="T21" t="s">
+      <c r="I44" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>